<commit_message>
Ajuste para subir a render
</commit_message>
<xml_diff>
--- a/resultados/resultados_dian.xlsx
+++ b/resultados/resultados_dian.xlsx
@@ -518,7 +518,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2025-05-05 08:49:54</t>
+          <t>2025-05-05 09:05:29</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -565,7 +565,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2025-05-05 08:50:03</t>
+          <t>2025-05-05 09:05:38</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -612,7 +612,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2025-05-05 08:50:10</t>
+          <t>2025-05-05 09:06:15</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">

</xml_diff>

<commit_message>
Ajuste de render para una vista agradable
</commit_message>
<xml_diff>
--- a/resultados/resultados_dian.xlsx
+++ b/resultados/resultados_dian.xlsx
@@ -518,7 +518,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2025-05-05 09:05:29</t>
+          <t>2025-05-05 11:18:12</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -535,42 +535,42 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>PROTECSA S.A. EN LIQUIDACION</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>No aplica</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>No aplica</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>No aplica</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>No aplica</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2025-05-05 09:05:38</t>
+          <t>2025-05-05 11:19:41</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>REGISTRO ACTIVO</t>
+          <t>Error de consulta o no registrado</t>
         </is>
       </c>
     </row>
@@ -582,42 +582,42 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>BANCO DE BOGOTA</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>No aplica</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>No aplica</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>No aplica</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>No aplica</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2025-05-05 09:06:15</t>
+          <t>2025-05-05 11:21:11</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>REGISTRO ACTIVO</t>
+          <t>Error de consulta o no registrado</t>
         </is>
       </c>
     </row>

</xml_diff>